<commit_message>
finished Relation and functions
</commit_message>
<xml_diff>
--- a/12/RelationsAndFunctions.xlsx
+++ b/12/RelationsAndFunctions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="162">
   <si>
     <t>1)</t>
   </si>
@@ -475,22 +475,50 @@
     <t>Composition of Functions</t>
   </si>
   <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>??</t>
+    <t>Check for One-to-One (injective)</t>
+  </si>
+  <si>
+    <t>Check for Onto (Surjective</t>
+  </si>
+  <si>
+    <t>condition of surjective is … for every output value, there should be one input value</t>
+  </si>
+  <si>
+    <t>Here N---&gt; N means domain is N and Range is N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 2 </t>
+  </si>
+  <si>
+    <t>f: Z---&gt; Z given by f(x) = square(x)</t>
+  </si>
+  <si>
+    <t>Now our set is real number (Z) and not natural nuber (N)</t>
+  </si>
+  <si>
+    <t>Check for Onto for part 2</t>
+  </si>
+  <si>
+    <t>f inverse function ----&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -521,8 +549,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -585,15 +614,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>145395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504826</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>115957</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>106432</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -611,8 +640,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2219326" y="23507701"/>
-          <a:ext cx="4286250" cy="2135256"/>
+          <a:off x="2009775" y="23195895"/>
+          <a:ext cx="5657849" cy="2818537"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -666,13 +695,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>133154</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -706,13 +735,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>11106</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -746,13 +775,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>441578</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -786,13 +815,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>125790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>221</xdr:row>
+      <xdr:row>248</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -826,13 +855,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>222</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>150910</xdr:colOff>
-      <xdr:row>236</xdr:row>
+      <xdr:row>263</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -866,13 +895,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>238</xdr:row>
+      <xdr:row>265</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>560416</xdr:colOff>
-      <xdr:row>251</xdr:row>
+      <xdr:row>278</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -893,6 +922,246 @@
         <a:xfrm>
           <a:off x="85725" y="45386625"/>
           <a:ext cx="4675216" cy="2590800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>14824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="781051" y="31828324"/>
+          <a:ext cx="4457699" cy="1385350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>88576</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4972050" y="30508575"/>
+          <a:ext cx="4117651" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>129972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7372351" y="32013526"/>
+          <a:ext cx="3657600" cy="1263446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>64938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1876425" y="34354938"/>
+          <a:ext cx="3419475" cy="1706711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>55477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7038976" y="34345477"/>
+          <a:ext cx="5200650" cy="1620923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>76923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1990726" y="53416923"/>
+          <a:ext cx="7867650" cy="2771052"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1163,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W257"/>
+  <dimension ref="A1:W284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="A285" sqref="A285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1883,22 +2152,110 @@
         <v>150</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
-      <c r="A169" t="s">
+    <row r="163" spans="3:17">
+      <c r="Q163" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="167" spans="3:17">
+      <c r="C167" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N167" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="168" spans="3:17">
+      <c r="M168" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="176" spans="3:17">
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="2:13">
+      <c r="C177" s="2"/>
+    </row>
+    <row r="178" spans="2:13">
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179" spans="2:13">
+      <c r="B179" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="2:13">
+      <c r="C180" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D180" s="2"/>
+      <c r="M180" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="181" spans="2:13">
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="2:13">
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="2:13">
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="2:13">
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="2:13">
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="2:13">
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="2:13">
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188" spans="2:13">
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189" spans="2:13">
+      <c r="C189" s="2"/>
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="2:13">
+      <c r="C190" s="2"/>
+      <c r="D190" s="2"/>
+    </row>
+    <row r="192" spans="2:13">
+      <c r="C192" s="2"/>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="D193" s="2"/>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
-      <c r="A179" t="s">
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
-      <c r="A257" t="s">
-        <v>153</v>
-      </c>
-      <c r="B257" t="s">
-        <v>154</v>
+    <row r="284" spans="1:1">
+      <c r="A284" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>